<commit_message>
Daten für ARD buffet Sendung hinzugefügt
</commit_message>
<xml_diff>
--- a/conversational_data_raw/data_source_overview.xlsx
+++ b/conversational_data_raw/data_source_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit - CookBERT\Github Repo\CookBERT\conversational_data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B935329-E9F8-4F97-8354-791EB13BE8FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C5758B-C272-4336-BB21-2931D22FB769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="132">
   <si>
     <t>Name</t>
   </si>
@@ -236,9 +236,6 @@
     <t>https://www.podcast.de/podcast/1096856/kochlust</t>
   </si>
   <si>
-    <t>keine Transkripte, deutsch</t>
-  </si>
-  <si>
     <t>Kochlust</t>
   </si>
   <si>
@@ -302,9 +299,6 @@
     <t>Sonstige</t>
   </si>
   <si>
-    <t>extrahiert</t>
-  </si>
-  <si>
     <t>Insta geschrieben</t>
   </si>
   <si>
@@ -336,12 +330,6 @@
   </si>
   <si>
     <t>ARD Buffet</t>
-  </si>
-  <si>
-    <t>Mehrere Folgen, jeweils so ca. 5 Minuten</t>
-  </si>
-  <si>
-    <t>muss noch extrahiert werden (mit JDownloader) | Beispieltranskript bereits heruntergeladen</t>
   </si>
   <si>
     <t>Status zu den Daten</t>
@@ -537,6 +525,23 @@
   </si>
   <si>
     <t>Email geschrieben</t>
+  </si>
+  <si>
+    <t>Ein Koch bereitet immer live ein Rezept zu, Moderator stellt dazu fragen.
+Daten sind die Untertitel von ARD und sind von unterschiedlich hoher qualität (manchmal fauler Transkriptor, der nur sinngemäß transkribiert, manchmal aber auch nahezu 1:1 Transkript)
+gutes Beispiel: sauerkrautsüppchen</t>
+  </si>
+  <si>
+    <t>ARD Kochshow, es wird immer 1 Rezept zubereitet und währenddessen über das Vorgehe diskutiert</t>
+  </si>
+  <si>
+    <t>Untertitel von 79 Sendungen (jeweils ca. 5 Minuten). Es wären noch mehr Sendungen verfügbar!</t>
+  </si>
+  <si>
+    <t>es können noch mehr daten gecrawled werden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Leute kochen live ein Rezept (etwas zusammengecuttet, sodass nur die wichtigen Stellen enthalten sind, wo gesprochen wird) und unterhalten sich währenddessen darüber/ erklären, was sie machen. </t>
   </si>
 </sst>
 </file>
@@ -698,7 +703,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
@@ -813,7 +818,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1098,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,6 +1119,7 @@
     <col min="4" max="6" width="25.7109375" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" style="5" customWidth="1"/>
     <col min="8" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
     <col min="12" max="12" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1125,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1134,30 +1143,30 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="270" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>13</v>
@@ -1170,7 +1179,7 @@
         <v>24</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J2" s="6"/>
     </row>
@@ -1179,7 +1188,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>19</v>
@@ -1196,7 +1205,7 @@
         <v>21</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J3" s="6"/>
     </row>
@@ -1205,7 +1214,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>15</v>
@@ -1218,25 +1227,25 @@
         <v>16</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>9</v>
@@ -1248,18 +1257,18 @@
         <v>22</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>11</v>
@@ -1268,7 +1277,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>10</v>
@@ -1277,45 +1286,45 @@
         <v>44513</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="22">
+      <c r="B7" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="21">
         <v>2</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="18" t="s">
+      <c r="E7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="14">
         <v>44513</v>
       </c>
-      <c r="H7" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>83</v>
+      <c r="H7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1323,16 +1332,16 @@
         <v>26</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D8" s="25">
         <v>2</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>25</v>
@@ -1341,13 +1350,13 @@
         <v>44513</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -1355,16 +1364,16 @@
         <v>30</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D9" s="28">
         <v>2</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>29</v>
@@ -1373,13 +1382,13 @@
         <v>44514</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="300" x14ac:dyDescent="0.25">
@@ -1387,16 +1396,16 @@
         <v>27</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D10" s="21">
         <v>2</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>28</v>
@@ -1405,13 +1414,13 @@
         <v>44514</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -1419,16 +1428,16 @@
         <v>32</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>31</v>
@@ -1437,13 +1446,13 @@
         <v>44514</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1451,16 +1460,16 @@
         <v>33</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D12" s="33">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>34</v>
@@ -1469,13 +1478,13 @@
         <v>44514</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -1483,16 +1492,16 @@
         <v>36</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D13" s="33">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F13" s="34" t="s">
         <v>35</v>
@@ -1501,13 +1510,13 @@
         <v>44514</v>
       </c>
       <c r="H13" s="32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I13" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J13" s="32" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1515,16 +1524,16 @@
         <v>38</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D14" s="33">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F14" s="34" t="s">
         <v>37</v>
@@ -1533,10 +1542,10 @@
         <v>44514</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" s="32" t="s">
         <v>39</v>
@@ -1547,31 +1556,31 @@
         <v>40</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D15" s="33">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G15" s="37">
         <v>44514</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -1579,10 +1588,10 @@
         <v>41</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D16" s="33">
         <v>2</v>
@@ -1597,30 +1606,30 @@
         <v>44514</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J16" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D17" s="33">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>44</v>
@@ -1629,150 +1638,163 @@
         <v>44514</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I17" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J17" s="32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C18" s="32"/>
+        <v>103</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>131</v>
+      </c>
       <c r="D18" s="33">
         <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="32" t="s">
         <v>48</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>47</v>
       </c>
       <c r="G18" s="37">
         <v>44514</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="I18" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="21"/>
+        <v>67</v>
+      </c>
+      <c r="D19" s="21">
+        <v>2</v>
+      </c>
       <c r="E19" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G19" s="15">
         <v>44513</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>77</v>
+    </row>
+    <row r="20" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="21">
+        <v>2</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="G20" s="42">
-        <v>44513</v>
-      </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>44514</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" s="43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="C21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" t="s">
+        <v>117</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>122</v>
       </c>
-      <c r="C21" t="s">
-        <v>119</v>
-      </c>
-      <c r="F21" t="s">
-        <v>117</v>
-      </c>
-      <c r="I21" s="32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="B23" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="40" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F22" t="s">
-        <v>121</v>
-      </c>
-      <c r="I22" s="32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>122</v>
-      </c>
-      <c r="E23" t="s">
-        <v>125</v>
-      </c>
-      <c r="F23" t="s">
-        <v>124</v>
-      </c>
       <c r="I23" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1792,9 +1814,10 @@
     <hyperlink ref="F14" r:id="rId13" xr:uid="{3A5CE10E-5F8B-49EF-AED1-FD741B60A7C7}"/>
     <hyperlink ref="F15" r:id="rId14" xr:uid="{9362C6C8-5079-45BF-A766-44E0F8F57754}"/>
     <hyperlink ref="F17" r:id="rId15" xr:uid="{63B88FD4-DFDC-46BC-B415-9F4286F565CF}"/>
+    <hyperlink ref="F18" r:id="rId16" xr:uid="{DBD597C3-F894-496B-B187-4FBD892C2EFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId17"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1828,32 +1851,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1876,37 +1899,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Citavi Projekt und related work hinzugefügt
</commit_message>
<xml_diff>
--- a/conversational_data_raw/data_source_overview.xlsx
+++ b/conversational_data_raw/data_source_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit - CookBERT\Github Repo\CookBERT\conversational_data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C5758B-C272-4336-BB21-2931D22FB769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00664686-7ACD-4382-BD12-6894215A5CC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -360,9 +360,6 @@
 Kein Transkript verfügbar</t>
   </si>
   <si>
-    <t>Kein Transkript/ Untertitel verfügbar</t>
-  </si>
-  <si>
     <t>6 Folgen, jeweils ca. 20 Minuten</t>
   </si>
   <si>
@@ -482,9 +479,6 @@
     <t>53 Folgen, jeweils ca. 25 Minuten</t>
   </si>
   <si>
-    <t>Email gesendet + auf Insta geschrieben</t>
-  </si>
-  <si>
     <t>https://www.br.de/mediathek/sendung/schuhbecks-av:584f4c2c3b467900117bfce7</t>
   </si>
   <si>
@@ -542,6 +536,9 @@
   </si>
   <si>
     <t xml:space="preserve">2 Leute kochen live ein Rezept (etwas zusammengecuttet, sodass nur die wichtigen Stellen enthalten sind, wo gesprochen wird) und unterhalten sich währenddessen darüber/ erklären, was sie machen. </t>
+  </si>
+  <si>
+    <t>Keine Textdaten verfügbar</t>
   </si>
 </sst>
 </file>
@@ -630,13 +627,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -703,7 +700,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
@@ -761,69 +758,73 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="6" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1108,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1246,7 @@
         <v>84</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>9</v>
@@ -1309,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>5</v>
@@ -1328,35 +1329,35 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="24" t="s">
+      <c r="B8" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="39">
         <v>2</v>
       </c>
-      <c r="E8" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="26" t="s">
+      <c r="E8" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="44">
         <v>44513</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="23" t="s">
-        <v>86</v>
+      <c r="J8" s="37" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -1367,22 +1368,22 @@
         <v>57</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="23">
+        <v>2</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="25">
+        <v>44514</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>88</v>
-      </c>
-      <c r="D9" s="28">
-        <v>2</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="30">
-        <v>44514</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>89</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>62</v>
@@ -1398,14 +1399,14 @@
       <c r="B10" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>90</v>
+      <c r="C10" s="26" t="s">
+        <v>89</v>
       </c>
       <c r="D10" s="21">
         <v>2</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>28</v>
@@ -1414,7 +1415,7 @@
         <v>44514</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>62</v>
@@ -1431,13 +1432,13 @@
         <v>57</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>99</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>31</v>
@@ -1446,7 +1447,7 @@
         <v>44514</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>62</v>
@@ -1456,227 +1457,227 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="28">
+        <v>2</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="30">
+        <v>44514</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="D13" s="28">
+        <v>2</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="32">
+        <v>44514</v>
+      </c>
+      <c r="H13" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="33">
+      <c r="I13" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="28">
         <v>2</v>
       </c>
-      <c r="E12" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="35">
+      <c r="E14" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="32">
         <v>44514</v>
       </c>
-      <c r="H12" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="I12" s="32" t="s">
+      <c r="H14" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="45" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="39">
+        <v>2</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="41">
+        <v>44514</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="32" t="s">
+      <c r="J15" s="37" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="45" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="37" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" s="33">
+      <c r="C16" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="39">
         <v>2</v>
       </c>
-      <c r="E13" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="37">
+      <c r="E16" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="41">
         <v>44514</v>
       </c>
-      <c r="H13" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="I13" s="32" t="s">
+      <c r="H16" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J13" s="32" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="33">
+      <c r="J16" s="42" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="28">
         <v>2</v>
       </c>
-      <c r="E14" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="37">
+      <c r="E17" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="32">
         <v>44514</v>
       </c>
-      <c r="H14" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="I14" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="195" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="33">
+      <c r="H17" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="28">
         <v>2</v>
       </c>
-      <c r="E15" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="37">
+      <c r="E18" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="32">
         <v>44514</v>
       </c>
-      <c r="H15" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="I15" s="32" t="s">
+      <c r="H18" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="I18" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="J15" s="32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="195" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="33">
-        <v>2</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="37">
-        <v>44514</v>
-      </c>
-      <c r="H16" s="32" t="s">
+      <c r="J18" s="27" t="s">
         <v>124</v>
-      </c>
-      <c r="I16" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" s="33">
-        <v>2</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="37">
-        <v>44514</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="I17" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" s="32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" s="33">
-        <v>2</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="37">
-        <v>44514</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="I18" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="J18" s="32" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1719,22 +1720,22 @@
         <v>55</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D20" s="21">
         <v>2</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="42">
+      <c r="G20" s="35">
         <v>44514</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>61</v>
@@ -1742,58 +1743,58 @@
       <c r="J20" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="K20" s="43" t="s">
-        <v>130</v>
+      <c r="K20" s="36" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" t="s">
+        <v>111</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B22" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" t="s">
         <v>115</v>
       </c>
-      <c r="F21" t="s">
-        <v>113</v>
-      </c>
-      <c r="I21" s="32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" t="s">
-        <v>117</v>
-      </c>
-      <c r="I22" s="32" t="s">
+      <c r="I22" s="27" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" t="s">
         <v>118</v>
       </c>
-      <c r="E23" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" t="s">
-        <v>120</v>
-      </c>
-      <c r="I23" s="32" t="s">
+      <c r="I23" s="27" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1929,7 +1930,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Untertitel zu weiteren Kochshows von ARD heruntergeladen
</commit_message>
<xml_diff>
--- a/conversational_data_raw/data_source_overview.xlsx
+++ b/conversational_data_raw/data_source_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit - CookBERT\Github Repo\CookBERT\conversational_data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F71871B-4AD6-4E30-B61A-0353515E2007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFBFCBA-089C-4F45-98D0-00AD80EFB9F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="151">
   <si>
     <t>Name</t>
   </si>
@@ -545,12 +545,69 @@
   <si>
     <t>https://www.ardmediathek.de/video/einfach-und-koestlich/polnisch-kochen-mit-agata-reul-s09-e08/wdr/Y3JpZDovL3dkci5kZS9CZWl0cmFnLTA4YzE2NzFkLTAxMjAtNGJiMC05NGE3LTg1NzExYzA3ZjRlNw/</t>
   </si>
+  <si>
+    <t>MDR um 4</t>
+  </si>
+  <si>
+    <t>https://www.ardmediathek.de/sendung/mdr-um-4/Y3JpZDovL21kci5kZS9zZW5kZXJlaWhlbi81MjU1MjUzNi05ODM5LTQwMWItODhlZi1iYTg2Y2EwMzA3Mjg/</t>
+  </si>
+  <si>
+    <t>36 Folgen, je ca. 10 mins</t>
+  </si>
+  <si>
+    <t>https://www.ardmediathek.de/suche/entenbrust/</t>
+  </si>
+  <si>
+    <t>unbedingt anschauen:</t>
+  </si>
+  <si>
+    <t>Wir in Bayern</t>
+  </si>
+  <si>
+    <t>https://www.ardmediathek.de/sendung/wir-in-bayern/Y3JpZDovL2JyLmRlL2Jyb2FkY2FzdFNlcmllcy9icm9hZGNhc3RTZXJpZXM6L2JyZGUvZmVybnNlaGVuL2JheWVyaXNjaGVzLWZlcm5zZWhlbi9zZW5kdW5nZW4vd2lyLWluLWJheWVybg/</t>
+  </si>
+  <si>
+    <t>https://www.ardmediathek.de/sendung/schleswig-holstein-magazin/Y3JpZDovL25kci5kZS8zNg/</t>
+  </si>
+  <si>
+    <t>Schleswig holstein magazin</t>
+  </si>
+  <si>
+    <t>https://www.ardmediathek.de/sendung/mein-nachmittag/Y3JpZDovL25kci5kZS8xMjQ1/</t>
+  </si>
+  <si>
+    <t>Mein nachmittag</t>
+  </si>
+  <si>
+    <t>https://www.ardmediathek.de/sendung/kaffee-oder-tee/Y3JpZDovL3N3ci5kZS8yMjQ0NDQ4/</t>
+  </si>
+  <si>
+    <t>Kaffee oder Tee</t>
+  </si>
+  <si>
+    <t>https://www.ardmediathek.de/sendung/einfach-gut-bachmeier/Y3JpZDovL2JyLmRlL2Jyb2FkY2FzdFNlcmllcy83NWNkM2IyMi00MzVmLTQ5N2EtOTNiNy0wNmJlZGNjOThmY2Y/</t>
+  </si>
+  <si>
+    <t>Einfach. Gut. Bachmeier</t>
+  </si>
+  <si>
+    <t>Kocht alleine!</t>
+  </si>
+  <si>
+    <t>Keine Untertitel verfügbar</t>
+  </si>
+  <si>
+    <t>108 Folgen</t>
+  </si>
+  <si>
+    <t>bis 14.07.2021</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,6 +657,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF343434"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -711,7 +775,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
@@ -848,6 +912,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1130,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,7 +1827,7 @@
         <v>74</v>
       </c>
       <c r="G20" s="34">
-        <v>44514</v>
+        <v>44519</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>122</v>
@@ -1822,8 +1894,120 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="C25" s="54" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="G26" s="51">
+        <v>44520</v>
+      </c>
+      <c r="H26" s="50"/>
+      <c r="I26" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" s="50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="5">
+        <v>44520</v>
+      </c>
+      <c r="I27" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F28" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="I28" t="s">
+        <v>61</v>
+      </c>
+      <c r="J28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="55"/>
+      <c r="E29" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="F29" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="G29" s="51">
+        <v>44520</v>
+      </c>
+      <c r="I29" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="J29" s="50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F30" s="54"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="I31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="53" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1845,9 +2029,14 @@
     <hyperlink ref="F17" r:id="rId15" xr:uid="{63B88FD4-DFDC-46BC-B415-9F4286F565CF}"/>
     <hyperlink ref="F18" r:id="rId16" xr:uid="{DBD597C3-F894-496B-B187-4FBD892C2EFF}"/>
     <hyperlink ref="F19" r:id="rId17" xr:uid="{639A3C54-10A0-4EC2-8472-12649880E73F}"/>
+    <hyperlink ref="C25" r:id="rId18" xr:uid="{356CADBE-1CD0-4446-95E9-B10374A990E9}"/>
+    <hyperlink ref="F27" r:id="rId19" xr:uid="{91F3B06E-9D6D-4011-B9AD-6EF63E8AB2AD}"/>
+    <hyperlink ref="F28" r:id="rId20" xr:uid="{A10D7378-793C-4C71-B0B9-014E6ACBAF6A}"/>
+    <hyperlink ref="F29" r:id="rId21" xr:uid="{629D217C-05B0-47BA-A069-9F82D35153BD}"/>
+    <hyperlink ref="F31" r:id="rId22" xr:uid="{EB1F2951-EEC0-4991-AF19-D839CA6535BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId23"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
Kaffee oder Tee Folgen vervollständigt
</commit_message>
<xml_diff>
--- a/conversational_data_raw/data_source_overview.xlsx
+++ b/conversational_data_raw/data_source_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit - CookBERT\Github Repo\CookBERT\conversational_data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFBFCBA-089C-4F45-98D0-00AD80EFB9F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5390DF9-1F17-47EA-B757-520085508F48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="151">
   <si>
     <t>Name</t>
   </si>
@@ -600,7 +600,7 @@
     <t>108 Folgen</t>
   </si>
   <si>
-    <t>bis 14.07.2021</t>
+    <t>335 Folgen</t>
   </si>
 </sst>
 </file>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,7 +1886,7 @@
       <c r="E23" t="s">
         <v>117</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="54" t="s">
         <v>116</v>
       </c>
       <c r="I23" s="27" t="s">
@@ -1978,17 +1978,27 @@
       <c r="F30" s="54"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="F31" s="54" t="s">
+      <c r="F31" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="I31" t="s">
+      <c r="G31" s="51">
+        <v>44520</v>
+      </c>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50" t="s">
         <v>61</v>
+      </c>
+      <c r="J31" s="50" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2034,9 +2044,10 @@
     <hyperlink ref="F28" r:id="rId20" xr:uid="{A10D7378-793C-4C71-B0B9-014E6ACBAF6A}"/>
     <hyperlink ref="F29" r:id="rId21" xr:uid="{629D217C-05B0-47BA-A069-9F82D35153BD}"/>
     <hyperlink ref="F31" r:id="rId22" xr:uid="{EB1F2951-EEC0-4991-AF19-D839CA6535BF}"/>
+    <hyperlink ref="F23" r:id="rId23" xr:uid="{6518593C-6D53-4E21-B5CC-785E916464C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId24"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>